<commit_message>
added load_time for completeness
</commit_message>
<xml_diff>
--- a/airline-data-dict-raw.xlsx
+++ b/airline-data-dict-raw.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="171">
   <si>
     <t>original_column_name</t>
   </si>
@@ -299,6 +299,24 @@
     <t>delay attribute to late aircraft</t>
   </si>
   <si>
+    <t>LOAD_TIME</t>
+  </si>
+  <si>
+    <t>load_time</t>
+  </si>
+  <si>
+    <t>timestamp that the raw data was loaded into BQ</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>2024-01-26 22:23:22.051288 UTC</t>
+  </si>
+  <si>
+    <t>UTC timestamp</t>
+  </si>
+  <si>
     <t>Code</t>
   </si>
   <si>
@@ -381,6 +399,9 @@
   </si>
   <si>
     <t>United states</t>
+  </si>
+  <si>
+    <t>TIMESTAMP</t>
   </si>
   <si>
     <t>meal_id</t>
@@ -537,7 +558,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/m/d"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="12">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -559,6 +580,18 @@
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <color theme="1"/>
@@ -641,6 +674,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -655,19 +694,17 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -677,14 +714,14 @@
     <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -927,7 +964,8 @@
     <col customWidth="1" min="2" max="2" width="25.88"/>
     <col customWidth="1" min="3" max="3" width="29.13"/>
     <col customWidth="1" min="4" max="4" width="12.63"/>
-    <col customWidth="1" min="5" max="6" width="23.88"/>
+    <col customWidth="1" min="5" max="5" width="34.13"/>
+    <col customWidth="1" min="6" max="6" width="23.88"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -2053,604 +2091,621 @@
       <c r="Z29" s="3"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="E30" s="8"/>
+      <c r="A30" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="E31" s="8"/>
+      <c r="E31" s="10"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="E32" s="8"/>
+      <c r="E32" s="10"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="E33" s="8"/>
+      <c r="E33" s="10"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="E34" s="8"/>
+      <c r="E34" s="10"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="E35" s="8"/>
+      <c r="E35" s="10"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="E36" s="8"/>
+      <c r="E36" s="10"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="E37" s="8"/>
+      <c r="E37" s="10"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="E38" s="8"/>
+      <c r="E38" s="10"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="E39" s="8"/>
+      <c r="E39" s="10"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="E40" s="8"/>
+      <c r="E40" s="10"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="E41" s="8"/>
+      <c r="E41" s="10"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="E42" s="8"/>
+      <c r="E42" s="10"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="E43" s="8"/>
+      <c r="E43" s="10"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="E44" s="8"/>
+      <c r="E44" s="10"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="E45" s="8"/>
+      <c r="E45" s="10"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="E46" s="8"/>
+      <c r="E46" s="10"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="E47" s="8"/>
+      <c r="E47" s="10"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="E48" s="8"/>
+      <c r="E48" s="10"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="E49" s="8"/>
+      <c r="E49" s="10"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="E50" s="8"/>
+      <c r="E50" s="10"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="E51" s="8"/>
+      <c r="E51" s="10"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="E52" s="8"/>
+      <c r="E52" s="10"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="E53" s="8"/>
+      <c r="E53" s="10"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="E54" s="8"/>
+      <c r="E54" s="10"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="E55" s="8"/>
+      <c r="E55" s="10"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="E56" s="8"/>
+      <c r="E56" s="10"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="E57" s="8"/>
+      <c r="E57" s="10"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="E58" s="8"/>
+      <c r="E58" s="10"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="E59" s="8"/>
+      <c r="E59" s="10"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="E60" s="8"/>
+      <c r="E60" s="10"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="E61" s="8"/>
+      <c r="E61" s="10"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="E62" s="8"/>
+      <c r="E62" s="10"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="E63" s="8"/>
+      <c r="E63" s="10"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="E64" s="8"/>
+      <c r="E64" s="10"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="E65" s="8"/>
+      <c r="E65" s="10"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="E66" s="8"/>
+      <c r="E66" s="10"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="E67" s="8"/>
+      <c r="E67" s="10"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="E68" s="8"/>
+      <c r="E68" s="10"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="E69" s="8"/>
+      <c r="E69" s="10"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="E70" s="8"/>
+      <c r="E70" s="10"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="E71" s="8"/>
+      <c r="E71" s="10"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="E72" s="8"/>
+      <c r="E72" s="10"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="E73" s="8"/>
+      <c r="E73" s="10"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="E74" s="8"/>
+      <c r="E74" s="10"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="E75" s="8"/>
+      <c r="E75" s="10"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="E76" s="8"/>
+      <c r="E76" s="10"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="E77" s="8"/>
+      <c r="E77" s="10"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="E78" s="8"/>
+      <c r="E78" s="10"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="E79" s="8"/>
+      <c r="E79" s="10"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="E80" s="8"/>
+      <c r="E80" s="10"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="E81" s="8"/>
+      <c r="E81" s="10"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="E82" s="8"/>
+      <c r="E82" s="10"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="E83" s="8"/>
+      <c r="E83" s="10"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="E84" s="8"/>
+      <c r="E84" s="10"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="E85" s="8"/>
+      <c r="E85" s="10"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="E86" s="8"/>
+      <c r="E86" s="10"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="E87" s="8"/>
+      <c r="E87" s="10"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="E88" s="8"/>
+      <c r="E88" s="10"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="E89" s="8"/>
+      <c r="E89" s="10"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="E90" s="8"/>
+      <c r="E90" s="10"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="E91" s="8"/>
+      <c r="E91" s="10"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="E92" s="8"/>
+      <c r="E92" s="10"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="E93" s="8"/>
+      <c r="E93" s="10"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="E94" s="8"/>
+      <c r="E94" s="10"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="E95" s="8"/>
+      <c r="E95" s="10"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="E96" s="8"/>
+      <c r="E96" s="10"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="E97" s="8"/>
+      <c r="E97" s="10"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="E98" s="8"/>
+      <c r="E98" s="10"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="E99" s="8"/>
+      <c r="E99" s="10"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="E100" s="8"/>
+      <c r="E100" s="10"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="E101" s="8"/>
+      <c r="E101" s="10"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="E102" s="8"/>
+      <c r="E102" s="10"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="E103" s="8"/>
+      <c r="E103" s="10"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="E104" s="8"/>
+      <c r="E104" s="10"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="E105" s="8"/>
+      <c r="E105" s="10"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="E106" s="8"/>
+      <c r="E106" s="10"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="E107" s="8"/>
+      <c r="E107" s="10"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="E108" s="8"/>
+      <c r="E108" s="10"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="E109" s="8"/>
+      <c r="E109" s="10"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="E110" s="8"/>
+      <c r="E110" s="10"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="E111" s="8"/>
+      <c r="E111" s="10"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="E112" s="8"/>
+      <c r="E112" s="10"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="E113" s="8"/>
+      <c r="E113" s="10"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="E114" s="8"/>
+      <c r="E114" s="10"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="E115" s="8"/>
+      <c r="E115" s="10"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="E116" s="8"/>
+      <c r="E116" s="10"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="E117" s="8"/>
+      <c r="E117" s="10"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="E118" s="8"/>
+      <c r="E118" s="10"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="E119" s="8"/>
+      <c r="E119" s="10"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="E120" s="8"/>
+      <c r="E120" s="10"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="E121" s="8"/>
+      <c r="E121" s="10"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="E122" s="8"/>
+      <c r="E122" s="10"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="E123" s="8"/>
+      <c r="E123" s="10"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="E124" s="8"/>
+      <c r="E124" s="10"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="E125" s="8"/>
+      <c r="E125" s="10"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="E126" s="8"/>
+      <c r="E126" s="10"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="E127" s="8"/>
+      <c r="E127" s="10"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="E128" s="8"/>
+      <c r="E128" s="10"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="E129" s="8"/>
+      <c r="E129" s="10"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="E130" s="8"/>
+      <c r="E130" s="10"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="E131" s="8"/>
+      <c r="E131" s="10"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="E132" s="8"/>
+      <c r="E132" s="10"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="E133" s="8"/>
+      <c r="E133" s="10"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="E134" s="8"/>
+      <c r="E134" s="10"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="E135" s="8"/>
+      <c r="E135" s="10"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="E136" s="8"/>
+      <c r="E136" s="10"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="E137" s="8"/>
+      <c r="E137" s="10"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="E138" s="8"/>
+      <c r="E138" s="10"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="E139" s="8"/>
+      <c r="E139" s="10"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="E140" s="8"/>
+      <c r="E140" s="10"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="E141" s="8"/>
+      <c r="E141" s="10"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="E142" s="8"/>
+      <c r="E142" s="10"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="E143" s="8"/>
+      <c r="E143" s="10"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="E144" s="8"/>
+      <c r="E144" s="10"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="E145" s="8"/>
+      <c r="E145" s="10"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="E146" s="8"/>
+      <c r="E146" s="10"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="E147" s="8"/>
+      <c r="E147" s="10"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="E148" s="8"/>
+      <c r="E148" s="10"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="E149" s="8"/>
+      <c r="E149" s="10"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="E150" s="8"/>
+      <c r="E150" s="10"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="E151" s="8"/>
+      <c r="E151" s="10"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="E152" s="8"/>
+      <c r="E152" s="10"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="E153" s="8"/>
+      <c r="E153" s="10"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="E154" s="8"/>
+      <c r="E154" s="10"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="E155" s="8"/>
+      <c r="E155" s="10"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="E156" s="8"/>
+      <c r="E156" s="10"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="E157" s="8"/>
+      <c r="E157" s="10"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="E158" s="8"/>
+      <c r="E158" s="10"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="E159" s="8"/>
+      <c r="E159" s="10"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="E160" s="8"/>
+      <c r="E160" s="10"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="E161" s="8"/>
+      <c r="E161" s="10"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="E162" s="8"/>
+      <c r="E162" s="10"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="E163" s="8"/>
+      <c r="E163" s="10"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="E164" s="8"/>
+      <c r="E164" s="10"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="E165" s="8"/>
+      <c r="E165" s="10"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="E166" s="8"/>
+      <c r="E166" s="10"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="E167" s="8"/>
+      <c r="E167" s="10"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="E168" s="8"/>
+      <c r="E168" s="10"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="E169" s="8"/>
+      <c r="E169" s="10"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="E170" s="8"/>
+      <c r="E170" s="10"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="E171" s="8"/>
+      <c r="E171" s="10"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="E172" s="8"/>
+      <c r="E172" s="10"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="E173" s="8"/>
+      <c r="E173" s="10"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="E174" s="8"/>
+      <c r="E174" s="10"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="E175" s="8"/>
+      <c r="E175" s="10"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="E176" s="8"/>
+      <c r="E176" s="10"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="E177" s="8"/>
+      <c r="E177" s="10"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="E178" s="8"/>
+      <c r="E178" s="10"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="E179" s="8"/>
+      <c r="E179" s="10"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="E180" s="8"/>
+      <c r="E180" s="10"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="E181" s="8"/>
+      <c r="E181" s="10"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="E182" s="8"/>
+      <c r="E182" s="10"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="E183" s="8"/>
+      <c r="E183" s="10"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="E184" s="8"/>
+      <c r="E184" s="10"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="E185" s="8"/>
+      <c r="E185" s="10"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="E186" s="8"/>
+      <c r="E186" s="10"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="E187" s="8"/>
+      <c r="E187" s="10"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="E188" s="8"/>
+      <c r="E188" s="10"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="E189" s="8"/>
+      <c r="E189" s="10"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="E190" s="8"/>
+      <c r="E190" s="10"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="E191" s="8"/>
+      <c r="E191" s="10"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="E192" s="8"/>
+      <c r="E192" s="10"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="E193" s="8"/>
+      <c r="E193" s="10"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="E194" s="8"/>
+      <c r="E194" s="10"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="E195" s="8"/>
+      <c r="E195" s="10"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="E196" s="8"/>
+      <c r="E196" s="10"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="E197" s="8"/>
+      <c r="E197" s="10"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="E198" s="8"/>
+      <c r="E198" s="10"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="E199" s="8"/>
+      <c r="E199" s="10"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="E200" s="8"/>
+      <c r="E200" s="10"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="E201" s="8"/>
+      <c r="E201" s="10"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="E202" s="8"/>
+      <c r="E202" s="10"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="E203" s="8"/>
+      <c r="E203" s="10"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="E204" s="8"/>
+      <c r="E204" s="10"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="E205" s="8"/>
+      <c r="E205" s="10"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="E206" s="8"/>
+      <c r="E206" s="10"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="E207" s="8"/>
+      <c r="E207" s="10"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="E208" s="8"/>
+      <c r="E208" s="10"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="E209" s="8"/>
+      <c r="E209" s="10"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="E210" s="8"/>
+      <c r="E210" s="10"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="E211" s="8"/>
+      <c r="E211" s="10"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="E212" s="8"/>
+      <c r="E212" s="10"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="E213" s="8"/>
+      <c r="E213" s="10"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="E214" s="8"/>
+      <c r="E214" s="10"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="E215" s="8"/>
+      <c r="E215" s="10"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="E216" s="8"/>
+      <c r="E216" s="10"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="E217" s="8"/>
+      <c r="E217" s="10"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="E218" s="8"/>
+      <c r="E218" s="10"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="E219" s="8"/>
+      <c r="E219" s="10"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="E220" s="8"/>
+      <c r="E220" s="10"/>
     </row>
     <row r="221" ht="15.75" customHeight="1">
-      <c r="E221" s="8"/>
+      <c r="E221" s="10"/>
     </row>
     <row r="222" ht="15.75" customHeight="1">
-      <c r="E222" s="8"/>
+      <c r="E222" s="10"/>
     </row>
     <row r="223" ht="15.75" customHeight="1">
-      <c r="E223" s="8"/>
+      <c r="E223" s="10"/>
     </row>
     <row r="224" ht="15.75" customHeight="1">
-      <c r="E224" s="8"/>
+      <c r="E224" s="10"/>
     </row>
     <row r="225" ht="15.75" customHeight="1">
-      <c r="E225" s="8"/>
+      <c r="E225" s="10"/>
     </row>
     <row r="226" ht="15.75" customHeight="1">
-      <c r="E226" s="8"/>
+      <c r="E226" s="10"/>
     </row>
     <row r="227" ht="15.75" customHeight="1">
-      <c r="E227" s="8"/>
+      <c r="E227" s="10"/>
     </row>
     <row r="228" ht="15.75" customHeight="1">
-      <c r="E228" s="8"/>
+      <c r="E228" s="10"/>
     </row>
     <row r="229" ht="15.75" customHeight="1">
-      <c r="E229" s="8"/>
+      <c r="E229" s="10"/>
     </row>
     <row r="230" ht="15.75" customHeight="1"/>
     <row r="231" ht="15.75" customHeight="1"/>
@@ -3447,22 +3502,22 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="3"/>
@@ -3487,22 +3542,22 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" s="12" t="s">
+      <c r="A2" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="5">
         <v>19805.0</v>
       </c>
-      <c r="F2" s="12"/>
+      <c r="F2" s="14"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -3525,22 +3580,22 @@
       <c r="Z2" s="3"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="D3" s="12" t="s">
+      <c r="A3" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="F3" s="12"/>
+        <v>99</v>
+      </c>
+      <c r="F3" s="14"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -3563,655 +3618,672 @@
       <c r="Z3" s="3"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="E4" s="8"/>
+      <c r="A4" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="E5" s="8"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="E6" s="8"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="E7" s="8"/>
+      <c r="E7" s="10"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="E8" s="8"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="E9" s="8"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="E10" s="8"/>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="E11" s="8"/>
+      <c r="E11" s="10"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="E12" s="8"/>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="E13" s="8"/>
+      <c r="E13" s="10"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="E14" s="8"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="E15" s="8"/>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="E16" s="8"/>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="E17" s="8"/>
+      <c r="E17" s="10"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="E18" s="8"/>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="E19" s="8"/>
+      <c r="E19" s="10"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="E20" s="8"/>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="E21" s="8"/>
+      <c r="E21" s="10"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="E22" s="8"/>
+      <c r="E22" s="10"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="E23" s="8"/>
+      <c r="E23" s="10"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="E24" s="8"/>
+      <c r="E24" s="10"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="E25" s="8"/>
+      <c r="E25" s="10"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="E26" s="8"/>
+      <c r="E26" s="10"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="E27" s="8"/>
+      <c r="E27" s="10"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="E28" s="8"/>
+      <c r="E28" s="10"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="E29" s="8"/>
+      <c r="E29" s="10"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="E30" s="8"/>
+      <c r="E30" s="10"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="E31" s="8"/>
+      <c r="E31" s="10"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="E32" s="8"/>
+      <c r="E32" s="10"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="E33" s="8"/>
+      <c r="E33" s="10"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="E34" s="8"/>
+      <c r="E34" s="10"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="E35" s="8"/>
+      <c r="E35" s="10"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="E36" s="8"/>
+      <c r="E36" s="10"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="E37" s="8"/>
+      <c r="E37" s="10"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="E38" s="8"/>
+      <c r="E38" s="10"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="E39" s="8"/>
+      <c r="E39" s="10"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="E40" s="8"/>
+      <c r="E40" s="10"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="E41" s="8"/>
+      <c r="E41" s="10"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="E42" s="8"/>
+      <c r="E42" s="10"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="E43" s="8"/>
+      <c r="E43" s="10"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="E44" s="8"/>
+      <c r="E44" s="10"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="E45" s="8"/>
+      <c r="E45" s="10"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="E46" s="8"/>
+      <c r="E46" s="10"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="E47" s="8"/>
+      <c r="E47" s="10"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="E48" s="8"/>
+      <c r="E48" s="10"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="E49" s="8"/>
+      <c r="E49" s="10"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="E50" s="8"/>
+      <c r="E50" s="10"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="E51" s="8"/>
+      <c r="E51" s="10"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="E52" s="8"/>
+      <c r="E52" s="10"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="E53" s="8"/>
+      <c r="E53" s="10"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="E54" s="8"/>
+      <c r="E54" s="10"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="E55" s="8"/>
+      <c r="E55" s="10"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="E56" s="8"/>
+      <c r="E56" s="10"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="E57" s="8"/>
+      <c r="E57" s="10"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="E58" s="8"/>
+      <c r="E58" s="10"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="E59" s="8"/>
+      <c r="E59" s="10"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="E60" s="8"/>
+      <c r="E60" s="10"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="E61" s="8"/>
+      <c r="E61" s="10"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="E62" s="8"/>
+      <c r="E62" s="10"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="E63" s="8"/>
+      <c r="E63" s="10"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="E64" s="8"/>
+      <c r="E64" s="10"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="E65" s="8"/>
+      <c r="E65" s="10"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="E66" s="8"/>
+      <c r="E66" s="10"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="E67" s="8"/>
+      <c r="E67" s="10"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="E68" s="8"/>
+      <c r="E68" s="10"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="E69" s="8"/>
+      <c r="E69" s="10"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="E70" s="8"/>
+      <c r="E70" s="10"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="E71" s="8"/>
+      <c r="E71" s="10"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="E72" s="8"/>
+      <c r="E72" s="10"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="E73" s="8"/>
+      <c r="E73" s="10"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="E74" s="8"/>
+      <c r="E74" s="10"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="E75" s="8"/>
+      <c r="E75" s="10"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="E76" s="8"/>
+      <c r="E76" s="10"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="E77" s="8"/>
+      <c r="E77" s="10"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="E78" s="8"/>
+      <c r="E78" s="10"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="E79" s="8"/>
+      <c r="E79" s="10"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="E80" s="8"/>
+      <c r="E80" s="10"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="E81" s="8"/>
+      <c r="E81" s="10"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="E82" s="8"/>
+      <c r="E82" s="10"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="E83" s="8"/>
+      <c r="E83" s="10"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="E84" s="8"/>
+      <c r="E84" s="10"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="E85" s="8"/>
+      <c r="E85" s="10"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="E86" s="8"/>
+      <c r="E86" s="10"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="E87" s="8"/>
+      <c r="E87" s="10"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="E88" s="8"/>
+      <c r="E88" s="10"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="E89" s="8"/>
+      <c r="E89" s="10"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="E90" s="8"/>
+      <c r="E90" s="10"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="E91" s="8"/>
+      <c r="E91" s="10"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="E92" s="8"/>
+      <c r="E92" s="10"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="E93" s="8"/>
+      <c r="E93" s="10"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="E94" s="8"/>
+      <c r="E94" s="10"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="E95" s="8"/>
+      <c r="E95" s="10"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="E96" s="8"/>
+      <c r="E96" s="10"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="E97" s="8"/>
+      <c r="E97" s="10"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="E98" s="8"/>
+      <c r="E98" s="10"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="E99" s="8"/>
+      <c r="E99" s="10"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="E100" s="8"/>
+      <c r="E100" s="10"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="E101" s="8"/>
+      <c r="E101" s="10"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="E102" s="8"/>
+      <c r="E102" s="10"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="E103" s="8"/>
+      <c r="E103" s="10"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="E104" s="8"/>
+      <c r="E104" s="10"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="E105" s="8"/>
+      <c r="E105" s="10"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="E106" s="8"/>
+      <c r="E106" s="10"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="E107" s="8"/>
+      <c r="E107" s="10"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="E108" s="8"/>
+      <c r="E108" s="10"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="E109" s="8"/>
+      <c r="E109" s="10"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="E110" s="8"/>
+      <c r="E110" s="10"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="E111" s="8"/>
+      <c r="E111" s="10"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="E112" s="8"/>
+      <c r="E112" s="10"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="E113" s="8"/>
+      <c r="E113" s="10"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="E114" s="8"/>
+      <c r="E114" s="10"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="E115" s="8"/>
+      <c r="E115" s="10"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="E116" s="8"/>
+      <c r="E116" s="10"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="E117" s="8"/>
+      <c r="E117" s="10"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="E118" s="8"/>
+      <c r="E118" s="10"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="E119" s="8"/>
+      <c r="E119" s="10"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="E120" s="8"/>
+      <c r="E120" s="10"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="E121" s="8"/>
+      <c r="E121" s="10"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="E122" s="8"/>
+      <c r="E122" s="10"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="E123" s="8"/>
+      <c r="E123" s="10"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="E124" s="8"/>
+      <c r="E124" s="10"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="E125" s="8"/>
+      <c r="E125" s="10"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="E126" s="8"/>
+      <c r="E126" s="10"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="E127" s="8"/>
+      <c r="E127" s="10"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="E128" s="8"/>
+      <c r="E128" s="10"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="E129" s="8"/>
+      <c r="E129" s="10"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="E130" s="8"/>
+      <c r="E130" s="10"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="E131" s="8"/>
+      <c r="E131" s="10"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="E132" s="8"/>
+      <c r="E132" s="10"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="E133" s="8"/>
+      <c r="E133" s="10"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="E134" s="8"/>
+      <c r="E134" s="10"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="E135" s="8"/>
+      <c r="E135" s="10"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="E136" s="8"/>
+      <c r="E136" s="10"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="E137" s="8"/>
+      <c r="E137" s="10"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="E138" s="8"/>
+      <c r="E138" s="10"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="E139" s="8"/>
+      <c r="E139" s="10"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="E140" s="8"/>
+      <c r="E140" s="10"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="E141" s="8"/>
+      <c r="E141" s="10"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="E142" s="8"/>
+      <c r="E142" s="10"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="E143" s="8"/>
+      <c r="E143" s="10"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="E144" s="8"/>
+      <c r="E144" s="10"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="E145" s="8"/>
+      <c r="E145" s="10"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="E146" s="8"/>
+      <c r="E146" s="10"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="E147" s="8"/>
+      <c r="E147" s="10"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="E148" s="8"/>
+      <c r="E148" s="10"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="E149" s="8"/>
+      <c r="E149" s="10"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="E150" s="8"/>
+      <c r="E150" s="10"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="E151" s="8"/>
+      <c r="E151" s="10"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="E152" s="8"/>
+      <c r="E152" s="10"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="E153" s="8"/>
+      <c r="E153" s="10"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="E154" s="8"/>
+      <c r="E154" s="10"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="E155" s="8"/>
+      <c r="E155" s="10"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="E156" s="8"/>
+      <c r="E156" s="10"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="E157" s="8"/>
+      <c r="E157" s="10"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="E158" s="8"/>
+      <c r="E158" s="10"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="E159" s="8"/>
+      <c r="E159" s="10"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="E160" s="8"/>
+      <c r="E160" s="10"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="E161" s="8"/>
+      <c r="E161" s="10"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="E162" s="8"/>
+      <c r="E162" s="10"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="E163" s="8"/>
+      <c r="E163" s="10"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="E164" s="8"/>
+      <c r="E164" s="10"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="E165" s="8"/>
+      <c r="E165" s="10"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="E166" s="8"/>
+      <c r="E166" s="10"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="E167" s="8"/>
+      <c r="E167" s="10"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="E168" s="8"/>
+      <c r="E168" s="10"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="E169" s="8"/>
+      <c r="E169" s="10"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="E170" s="8"/>
+      <c r="E170" s="10"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="E171" s="8"/>
+      <c r="E171" s="10"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="E172" s="8"/>
+      <c r="E172" s="10"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="E173" s="8"/>
+      <c r="E173" s="10"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="E174" s="8"/>
+      <c r="E174" s="10"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="E175" s="8"/>
+      <c r="E175" s="10"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="E176" s="8"/>
+      <c r="E176" s="10"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="E177" s="8"/>
+      <c r="E177" s="10"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="E178" s="8"/>
+      <c r="E178" s="10"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="E179" s="8"/>
+      <c r="E179" s="10"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="E180" s="8"/>
+      <c r="E180" s="10"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="E181" s="8"/>
+      <c r="E181" s="10"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="E182" s="8"/>
+      <c r="E182" s="10"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="E183" s="8"/>
+      <c r="E183" s="10"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="E184" s="8"/>
+      <c r="E184" s="10"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="E185" s="8"/>
+      <c r="E185" s="10"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="E186" s="8"/>
+      <c r="E186" s="10"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="E187" s="8"/>
+      <c r="E187" s="10"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="E188" s="8"/>
+      <c r="E188" s="10"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="E189" s="8"/>
+      <c r="E189" s="10"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="E190" s="8"/>
+      <c r="E190" s="10"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="E191" s="8"/>
+      <c r="E191" s="10"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="E192" s="8"/>
+      <c r="E192" s="10"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="E193" s="8"/>
+      <c r="E193" s="10"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="E194" s="8"/>
+      <c r="E194" s="10"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="E195" s="8"/>
+      <c r="E195" s="10"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="E196" s="8"/>
+      <c r="E196" s="10"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="E197" s="8"/>
+      <c r="E197" s="10"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="E198" s="8"/>
+      <c r="E198" s="10"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="E199" s="8"/>
+      <c r="E199" s="10"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="E200" s="8"/>
+      <c r="E200" s="10"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="E201" s="8"/>
+      <c r="E201" s="10"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="E202" s="8"/>
+      <c r="E202" s="10"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="E203" s="8"/>
+      <c r="E203" s="10"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="E204" s="8"/>
+      <c r="E204" s="10"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="E205" s="8"/>
+      <c r="E205" s="10"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="E206" s="8"/>
+      <c r="E206" s="10"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="E207" s="8"/>
+      <c r="E207" s="10"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="E208" s="8"/>
+      <c r="E208" s="10"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="E209" s="8"/>
+      <c r="E209" s="10"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="E210" s="8"/>
+      <c r="E210" s="10"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="E211" s="8"/>
+      <c r="E211" s="10"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="E212" s="8"/>
+      <c r="E212" s="10"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="E213" s="8"/>
+      <c r="E213" s="10"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="E214" s="8"/>
+      <c r="E214" s="10"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="E215" s="8"/>
+      <c r="E215" s="10"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="E216" s="8"/>
+      <c r="E216" s="10"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="E217" s="8"/>
+      <c r="E217" s="10"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="E218" s="8"/>
+      <c r="E218" s="10"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="E219" s="8"/>
+      <c r="E219" s="10"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="E220" s="8"/>
+      <c r="E220" s="10"/>
     </row>
     <row r="221" ht="15.75" customHeight="1"/>
     <row r="222" ht="15.75" customHeight="1"/>
@@ -5017,23 +5089,23 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="11" t="s">
-        <v>94</v>
+      <c r="F1" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -5057,22 +5129,22 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="D2" s="12" t="s">
+      <c r="A2" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2" s="14" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F2" s="12"/>
+        <v>102</v>
+      </c>
+      <c r="F2" s="14"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -5095,23 +5167,23 @@
       <c r="Z2" s="3"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
-      <c r="A3" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" s="12" t="s">
+      <c r="A3" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="C3" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>99</v>
+        <v>104</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>105</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -5135,655 +5207,672 @@
       <c r="Z3" s="3"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
-      <c r="E4" s="8"/>
+      <c r="A4" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="E5" s="8"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="E6" s="8"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="E7" s="8"/>
+      <c r="E7" s="10"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="E8" s="8"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="E9" s="8"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="E10" s="8"/>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="E11" s="8"/>
+      <c r="E11" s="10"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="E12" s="8"/>
+      <c r="E12" s="10"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="E13" s="8"/>
+      <c r="E13" s="10"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="E14" s="8"/>
+      <c r="E14" s="10"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="E15" s="8"/>
+      <c r="E15" s="10"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="E16" s="8"/>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="E17" s="8"/>
+      <c r="E17" s="10"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="E18" s="8"/>
+      <c r="E18" s="10"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="E19" s="8"/>
+      <c r="E19" s="10"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="E20" s="8"/>
+      <c r="E20" s="10"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="E21" s="8"/>
+      <c r="E21" s="10"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="E22" s="8"/>
+      <c r="E22" s="10"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="E23" s="8"/>
+      <c r="E23" s="10"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="E24" s="8"/>
+      <c r="E24" s="10"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="E25" s="8"/>
+      <c r="E25" s="10"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="E26" s="8"/>
+      <c r="E26" s="10"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="E27" s="8"/>
+      <c r="E27" s="10"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="E28" s="8"/>
+      <c r="E28" s="10"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="E29" s="8"/>
+      <c r="E29" s="10"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="E30" s="8"/>
+      <c r="E30" s="10"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="E31" s="8"/>
+      <c r="E31" s="10"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="E32" s="8"/>
+      <c r="E32" s="10"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="E33" s="8"/>
+      <c r="E33" s="10"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="E34" s="8"/>
+      <c r="E34" s="10"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="E35" s="8"/>
+      <c r="E35" s="10"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="E36" s="8"/>
+      <c r="E36" s="10"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="E37" s="8"/>
+      <c r="E37" s="10"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="E38" s="8"/>
+      <c r="E38" s="10"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="E39" s="8"/>
+      <c r="E39" s="10"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="E40" s="8"/>
+      <c r="E40" s="10"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="E41" s="8"/>
+      <c r="E41" s="10"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="E42" s="8"/>
+      <c r="E42" s="10"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="E43" s="8"/>
+      <c r="E43" s="10"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="E44" s="8"/>
+      <c r="E44" s="10"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="E45" s="8"/>
+      <c r="E45" s="10"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="E46" s="8"/>
+      <c r="E46" s="10"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="E47" s="8"/>
+      <c r="E47" s="10"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="E48" s="8"/>
+      <c r="E48" s="10"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="E49" s="8"/>
+      <c r="E49" s="10"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="E50" s="8"/>
+      <c r="E50" s="10"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="E51" s="8"/>
+      <c r="E51" s="10"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="E52" s="8"/>
+      <c r="E52" s="10"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="E53" s="8"/>
+      <c r="E53" s="10"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="E54" s="8"/>
+      <c r="E54" s="10"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="E55" s="8"/>
+      <c r="E55" s="10"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="E56" s="8"/>
+      <c r="E56" s="10"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="E57" s="8"/>
+      <c r="E57" s="10"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="E58" s="8"/>
+      <c r="E58" s="10"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="E59" s="8"/>
+      <c r="E59" s="10"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="E60" s="8"/>
+      <c r="E60" s="10"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="E61" s="8"/>
+      <c r="E61" s="10"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="E62" s="8"/>
+      <c r="E62" s="10"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="E63" s="8"/>
+      <c r="E63" s="10"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="E64" s="8"/>
+      <c r="E64" s="10"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="E65" s="8"/>
+      <c r="E65" s="10"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="E66" s="8"/>
+      <c r="E66" s="10"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="E67" s="8"/>
+      <c r="E67" s="10"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="E68" s="8"/>
+      <c r="E68" s="10"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="E69" s="8"/>
+      <c r="E69" s="10"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="E70" s="8"/>
+      <c r="E70" s="10"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="E71" s="8"/>
+      <c r="E71" s="10"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="E72" s="8"/>
+      <c r="E72" s="10"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="E73" s="8"/>
+      <c r="E73" s="10"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="E74" s="8"/>
+      <c r="E74" s="10"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="E75" s="8"/>
+      <c r="E75" s="10"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="E76" s="8"/>
+      <c r="E76" s="10"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="E77" s="8"/>
+      <c r="E77" s="10"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="E78" s="8"/>
+      <c r="E78" s="10"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="E79" s="8"/>
+      <c r="E79" s="10"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="E80" s="8"/>
+      <c r="E80" s="10"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="E81" s="8"/>
+      <c r="E81" s="10"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="E82" s="8"/>
+      <c r="E82" s="10"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="E83" s="8"/>
+      <c r="E83" s="10"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="E84" s="8"/>
+      <c r="E84" s="10"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="E85" s="8"/>
+      <c r="E85" s="10"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="E86" s="8"/>
+      <c r="E86" s="10"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="E87" s="8"/>
+      <c r="E87" s="10"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="E88" s="8"/>
+      <c r="E88" s="10"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="E89" s="8"/>
+      <c r="E89" s="10"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="E90" s="8"/>
+      <c r="E90" s="10"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="E91" s="8"/>
+      <c r="E91" s="10"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="E92" s="8"/>
+      <c r="E92" s="10"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="E93" s="8"/>
+      <c r="E93" s="10"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="E94" s="8"/>
+      <c r="E94" s="10"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="E95" s="8"/>
+      <c r="E95" s="10"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="E96" s="8"/>
+      <c r="E96" s="10"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="E97" s="8"/>
+      <c r="E97" s="10"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="E98" s="8"/>
+      <c r="E98" s="10"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="E99" s="8"/>
+      <c r="E99" s="10"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="E100" s="8"/>
+      <c r="E100" s="10"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="E101" s="8"/>
+      <c r="E101" s="10"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="E102" s="8"/>
+      <c r="E102" s="10"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="E103" s="8"/>
+      <c r="E103" s="10"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="E104" s="8"/>
+      <c r="E104" s="10"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="E105" s="8"/>
+      <c r="E105" s="10"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="E106" s="8"/>
+      <c r="E106" s="10"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="E107" s="8"/>
+      <c r="E107" s="10"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="E108" s="8"/>
+      <c r="E108" s="10"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="E109" s="8"/>
+      <c r="E109" s="10"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="E110" s="8"/>
+      <c r="E110" s="10"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="E111" s="8"/>
+      <c r="E111" s="10"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="E112" s="8"/>
+      <c r="E112" s="10"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="E113" s="8"/>
+      <c r="E113" s="10"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="E114" s="8"/>
+      <c r="E114" s="10"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="E115" s="8"/>
+      <c r="E115" s="10"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="E116" s="8"/>
+      <c r="E116" s="10"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="E117" s="8"/>
+      <c r="E117" s="10"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="E118" s="8"/>
+      <c r="E118" s="10"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="E119" s="8"/>
+      <c r="E119" s="10"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="E120" s="8"/>
+      <c r="E120" s="10"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="E121" s="8"/>
+      <c r="E121" s="10"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="E122" s="8"/>
+      <c r="E122" s="10"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="E123" s="8"/>
+      <c r="E123" s="10"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="E124" s="8"/>
+      <c r="E124" s="10"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="E125" s="8"/>
+      <c r="E125" s="10"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="E126" s="8"/>
+      <c r="E126" s="10"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="E127" s="8"/>
+      <c r="E127" s="10"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="E128" s="8"/>
+      <c r="E128" s="10"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="E129" s="8"/>
+      <c r="E129" s="10"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="E130" s="8"/>
+      <c r="E130" s="10"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="E131" s="8"/>
+      <c r="E131" s="10"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="E132" s="8"/>
+      <c r="E132" s="10"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="E133" s="8"/>
+      <c r="E133" s="10"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="E134" s="8"/>
+      <c r="E134" s="10"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="E135" s="8"/>
+      <c r="E135" s="10"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="E136" s="8"/>
+      <c r="E136" s="10"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="E137" s="8"/>
+      <c r="E137" s="10"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="E138" s="8"/>
+      <c r="E138" s="10"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="E139" s="8"/>
+      <c r="E139" s="10"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="E140" s="8"/>
+      <c r="E140" s="10"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="E141" s="8"/>
+      <c r="E141" s="10"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="E142" s="8"/>
+      <c r="E142" s="10"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="E143" s="8"/>
+      <c r="E143" s="10"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="E144" s="8"/>
+      <c r="E144" s="10"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="E145" s="8"/>
+      <c r="E145" s="10"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="E146" s="8"/>
+      <c r="E146" s="10"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="E147" s="8"/>
+      <c r="E147" s="10"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="E148" s="8"/>
+      <c r="E148" s="10"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="E149" s="8"/>
+      <c r="E149" s="10"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="E150" s="8"/>
+      <c r="E150" s="10"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="E151" s="8"/>
+      <c r="E151" s="10"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="E152" s="8"/>
+      <c r="E152" s="10"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="E153" s="8"/>
+      <c r="E153" s="10"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="E154" s="8"/>
+      <c r="E154" s="10"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="E155" s="8"/>
+      <c r="E155" s="10"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="E156" s="8"/>
+      <c r="E156" s="10"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="E157" s="8"/>
+      <c r="E157" s="10"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="E158" s="8"/>
+      <c r="E158" s="10"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="E159" s="8"/>
+      <c r="E159" s="10"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="E160" s="8"/>
+      <c r="E160" s="10"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="E161" s="8"/>
+      <c r="E161" s="10"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="E162" s="8"/>
+      <c r="E162" s="10"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="E163" s="8"/>
+      <c r="E163" s="10"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="E164" s="8"/>
+      <c r="E164" s="10"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="E165" s="8"/>
+      <c r="E165" s="10"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="E166" s="8"/>
+      <c r="E166" s="10"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="E167" s="8"/>
+      <c r="E167" s="10"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="E168" s="8"/>
+      <c r="E168" s="10"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="E169" s="8"/>
+      <c r="E169" s="10"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="E170" s="8"/>
+      <c r="E170" s="10"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="E171" s="8"/>
+      <c r="E171" s="10"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="E172" s="8"/>
+      <c r="E172" s="10"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="E173" s="8"/>
+      <c r="E173" s="10"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="E174" s="8"/>
+      <c r="E174" s="10"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="E175" s="8"/>
+      <c r="E175" s="10"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="E176" s="8"/>
+      <c r="E176" s="10"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="E177" s="8"/>
+      <c r="E177" s="10"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="E178" s="8"/>
+      <c r="E178" s="10"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="E179" s="8"/>
+      <c r="E179" s="10"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="E180" s="8"/>
+      <c r="E180" s="10"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="E181" s="8"/>
+      <c r="E181" s="10"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="E182" s="8"/>
+      <c r="E182" s="10"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="E183" s="8"/>
+      <c r="E183" s="10"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="E184" s="8"/>
+      <c r="E184" s="10"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="E185" s="8"/>
+      <c r="E185" s="10"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="E186" s="8"/>
+      <c r="E186" s="10"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="E187" s="8"/>
+      <c r="E187" s="10"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="E188" s="8"/>
+      <c r="E188" s="10"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="E189" s="8"/>
+      <c r="E189" s="10"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="E190" s="8"/>
+      <c r="E190" s="10"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="E191" s="8"/>
+      <c r="E191" s="10"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="E192" s="8"/>
+      <c r="E192" s="10"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="E193" s="8"/>
+      <c r="E193" s="10"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="E194" s="8"/>
+      <c r="E194" s="10"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="E195" s="8"/>
+      <c r="E195" s="10"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="E196" s="8"/>
+      <c r="E196" s="10"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="E197" s="8"/>
+      <c r="E197" s="10"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="E198" s="8"/>
+      <c r="E198" s="10"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="E199" s="8"/>
+      <c r="E199" s="10"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="E200" s="8"/>
+      <c r="E200" s="10"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="E201" s="8"/>
+      <c r="E201" s="10"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="E202" s="8"/>
+      <c r="E202" s="10"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="E203" s="8"/>
+      <c r="E203" s="10"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="E204" s="8"/>
+      <c r="E204" s="10"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="E205" s="8"/>
+      <c r="E205" s="10"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="E206" s="8"/>
+      <c r="E206" s="10"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="E207" s="8"/>
+      <c r="E207" s="10"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="E208" s="8"/>
+      <c r="E208" s="10"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="E209" s="8"/>
+      <c r="E209" s="10"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="E210" s="8"/>
+      <c r="E210" s="10"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="E211" s="8"/>
+      <c r="E211" s="10"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="E212" s="8"/>
+      <c r="E212" s="10"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="E213" s="8"/>
+      <c r="E213" s="10"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="E214" s="8"/>
+      <c r="E214" s="10"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="E215" s="8"/>
+      <c r="E215" s="10"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="E216" s="8"/>
+      <c r="E216" s="10"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="E217" s="8"/>
+      <c r="E217" s="10"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="E218" s="8"/>
+      <c r="E218" s="10"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="E219" s="8"/>
+      <c r="E219" s="10"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="E220" s="8"/>
+      <c r="E220" s="10"/>
     </row>
     <row r="221" ht="15.75" customHeight="1"/>
     <row r="222" ht="15.75" customHeight="1"/>
@@ -6582,22 +6671,22 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="14.0"/>
     <col customWidth="1" min="2" max="2" width="12.63"/>
-    <col customWidth="1" min="3" max="3" width="25.5"/>
+    <col customWidth="1" min="3" max="3" width="29.63"/>
     <col customWidth="1" min="4" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
@@ -6624,16 +6713,16 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>103</v>
+        <v>108</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>109</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -6660,13 +6749,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>106</v>
+        <v>108</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>112</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -6694,13 +6783,13 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="13" t="s">
         <v>108</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>114</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -6728,13 +6817,13 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>110</v>
+        <v>108</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>116</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -6762,13 +6851,13 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>112</v>
+        <v>108</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>118</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -6796,13 +6885,13 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>114</v>
+        <v>108</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>120</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -6828,7 +6917,20 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1"/>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
     <row r="9" ht="15.75" customHeight="1"/>
     <row r="10" ht="15.75" customHeight="1"/>
     <row r="11" ht="15.75" customHeight="1"/>
@@ -7843,11 +7945,11 @@
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>4</v>
@@ -7877,10 +7979,10 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="C2" s="15">
         <v>52874.0</v>
@@ -7910,13 +8012,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -7943,13 +8045,13 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -7976,13 +8078,13 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -8009,13 +8111,13 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -8042,13 +8144,13 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -8075,13 +8177,13 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -8108,13 +8210,13 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -8141,13 +8243,13 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -8174,13 +8276,13 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -8207,13 +8309,13 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -8240,13 +8342,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -8273,13 +8375,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -8305,622 +8407,631 @@
       <c r="Y14" s="3"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="C15" s="8"/>
+      <c r="A15" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="8"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="C16" s="8"/>
+      <c r="C16" s="10"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="C17" s="8"/>
+      <c r="C17" s="10"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="C18" s="8"/>
+      <c r="C18" s="10"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="C19" s="8"/>
+      <c r="C19" s="10"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="C20" s="8"/>
+      <c r="C20" s="10"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="C21" s="8"/>
+      <c r="C21" s="10"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="C22" s="8"/>
+      <c r="C22" s="10"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="C23" s="8"/>
+      <c r="C23" s="10"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="C24" s="8"/>
+      <c r="C24" s="10"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="C25" s="8"/>
+      <c r="C25" s="10"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="C26" s="8"/>
+      <c r="C26" s="10"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="C27" s="8"/>
+      <c r="C27" s="10"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="C28" s="8"/>
+      <c r="C28" s="10"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="C29" s="8"/>
+      <c r="C29" s="10"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="C30" s="8"/>
+      <c r="C30" s="10"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="C31" s="8"/>
+      <c r="C31" s="10"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="C32" s="8"/>
+      <c r="C32" s="10"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="C33" s="8"/>
+      <c r="C33" s="10"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="C34" s="8"/>
+      <c r="C34" s="10"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="C35" s="8"/>
+      <c r="C35" s="10"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="C36" s="8"/>
+      <c r="C36" s="10"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="C37" s="8"/>
+      <c r="C37" s="10"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="C38" s="8"/>
+      <c r="C38" s="10"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="C39" s="8"/>
+      <c r="C39" s="10"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="C40" s="8"/>
+      <c r="C40" s="10"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="C41" s="8"/>
+      <c r="C41" s="10"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="C42" s="8"/>
+      <c r="C42" s="10"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="C43" s="8"/>
+      <c r="C43" s="10"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="C44" s="8"/>
+      <c r="C44" s="10"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="C45" s="8"/>
+      <c r="C45" s="10"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="C46" s="8"/>
+      <c r="C46" s="10"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="C47" s="8"/>
+      <c r="C47" s="10"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="C48" s="8"/>
+      <c r="C48" s="10"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="C49" s="8"/>
+      <c r="C49" s="10"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="C50" s="8"/>
+      <c r="C50" s="10"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="C51" s="8"/>
+      <c r="C51" s="10"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="C52" s="8"/>
+      <c r="C52" s="10"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="C53" s="8"/>
+      <c r="C53" s="10"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="C54" s="8"/>
+      <c r="C54" s="10"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="C55" s="8"/>
+      <c r="C55" s="10"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="C56" s="8"/>
+      <c r="C56" s="10"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="C57" s="8"/>
+      <c r="C57" s="10"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="C58" s="8"/>
+      <c r="C58" s="10"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="C59" s="8"/>
+      <c r="C59" s="10"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="C60" s="8"/>
+      <c r="C60" s="10"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="C61" s="8"/>
+      <c r="C61" s="10"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="C62" s="8"/>
+      <c r="C62" s="10"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="C63" s="8"/>
+      <c r="C63" s="10"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="C64" s="8"/>
+      <c r="C64" s="10"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="C65" s="8"/>
+      <c r="C65" s="10"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="C66" s="8"/>
+      <c r="C66" s="10"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="C67" s="8"/>
+      <c r="C67" s="10"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="C68" s="8"/>
+      <c r="C68" s="10"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="C69" s="8"/>
+      <c r="C69" s="10"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="C70" s="8"/>
+      <c r="C70" s="10"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="C71" s="8"/>
+      <c r="C71" s="10"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="C72" s="8"/>
+      <c r="C72" s="10"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="C73" s="8"/>
+      <c r="C73" s="10"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="C74" s="8"/>
+      <c r="C74" s="10"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="C75" s="8"/>
+      <c r="C75" s="10"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="C76" s="8"/>
+      <c r="C76" s="10"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="C77" s="8"/>
+      <c r="C77" s="10"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="C78" s="8"/>
+      <c r="C78" s="10"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="C79" s="8"/>
+      <c r="C79" s="10"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="C80" s="8"/>
+      <c r="C80" s="10"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="C81" s="8"/>
+      <c r="C81" s="10"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="C82" s="8"/>
+      <c r="C82" s="10"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="C83" s="8"/>
+      <c r="C83" s="10"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="C84" s="8"/>
+      <c r="C84" s="10"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="C85" s="8"/>
+      <c r="C85" s="10"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="C86" s="8"/>
+      <c r="C86" s="10"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="C87" s="8"/>
+      <c r="C87" s="10"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="C88" s="8"/>
+      <c r="C88" s="10"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="C89" s="8"/>
+      <c r="C89" s="10"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="C90" s="8"/>
+      <c r="C90" s="10"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="C91" s="8"/>
+      <c r="C91" s="10"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="C92" s="8"/>
+      <c r="C92" s="10"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="C93" s="8"/>
+      <c r="C93" s="10"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="C94" s="8"/>
+      <c r="C94" s="10"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="C95" s="8"/>
+      <c r="C95" s="10"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="C96" s="8"/>
+      <c r="C96" s="10"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="C97" s="8"/>
+      <c r="C97" s="10"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="C98" s="8"/>
+      <c r="C98" s="10"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="C99" s="8"/>
+      <c r="C99" s="10"/>
     </row>
     <row r="100" ht="15.75" customHeight="1">
-      <c r="C100" s="8"/>
+      <c r="C100" s="10"/>
     </row>
     <row r="101" ht="15.75" customHeight="1">
-      <c r="C101" s="8"/>
+      <c r="C101" s="10"/>
     </row>
     <row r="102" ht="15.75" customHeight="1">
-      <c r="C102" s="8"/>
+      <c r="C102" s="10"/>
     </row>
     <row r="103" ht="15.75" customHeight="1">
-      <c r="C103" s="8"/>
+      <c r="C103" s="10"/>
     </row>
     <row r="104" ht="15.75" customHeight="1">
-      <c r="C104" s="8"/>
+      <c r="C104" s="10"/>
     </row>
     <row r="105" ht="15.75" customHeight="1">
-      <c r="C105" s="8"/>
+      <c r="C105" s="10"/>
     </row>
     <row r="106" ht="15.75" customHeight="1">
-      <c r="C106" s="8"/>
+      <c r="C106" s="10"/>
     </row>
     <row r="107" ht="15.75" customHeight="1">
-      <c r="C107" s="8"/>
+      <c r="C107" s="10"/>
     </row>
     <row r="108" ht="15.75" customHeight="1">
-      <c r="C108" s="8"/>
+      <c r="C108" s="10"/>
     </row>
     <row r="109" ht="15.75" customHeight="1">
-      <c r="C109" s="8"/>
+      <c r="C109" s="10"/>
     </row>
     <row r="110" ht="15.75" customHeight="1">
-      <c r="C110" s="8"/>
+      <c r="C110" s="10"/>
     </row>
     <row r="111" ht="15.75" customHeight="1">
-      <c r="C111" s="8"/>
+      <c r="C111" s="10"/>
     </row>
     <row r="112" ht="15.75" customHeight="1">
-      <c r="C112" s="8"/>
+      <c r="C112" s="10"/>
     </row>
     <row r="113" ht="15.75" customHeight="1">
-      <c r="C113" s="8"/>
+      <c r="C113" s="10"/>
     </row>
     <row r="114" ht="15.75" customHeight="1">
-      <c r="C114" s="8"/>
+      <c r="C114" s="10"/>
     </row>
     <row r="115" ht="15.75" customHeight="1">
-      <c r="C115" s="8"/>
+      <c r="C115" s="10"/>
     </row>
     <row r="116" ht="15.75" customHeight="1">
-      <c r="C116" s="8"/>
+      <c r="C116" s="10"/>
     </row>
     <row r="117" ht="15.75" customHeight="1">
-      <c r="C117" s="8"/>
+      <c r="C117" s="10"/>
     </row>
     <row r="118" ht="15.75" customHeight="1">
-      <c r="C118" s="8"/>
+      <c r="C118" s="10"/>
     </row>
     <row r="119" ht="15.75" customHeight="1">
-      <c r="C119" s="8"/>
+      <c r="C119" s="10"/>
     </row>
     <row r="120" ht="15.75" customHeight="1">
-      <c r="C120" s="8"/>
+      <c r="C120" s="10"/>
     </row>
     <row r="121" ht="15.75" customHeight="1">
-      <c r="C121" s="8"/>
+      <c r="C121" s="10"/>
     </row>
     <row r="122" ht="15.75" customHeight="1">
-      <c r="C122" s="8"/>
+      <c r="C122" s="10"/>
     </row>
     <row r="123" ht="15.75" customHeight="1">
-      <c r="C123" s="8"/>
+      <c r="C123" s="10"/>
     </row>
     <row r="124" ht="15.75" customHeight="1">
-      <c r="C124" s="8"/>
+      <c r="C124" s="10"/>
     </row>
     <row r="125" ht="15.75" customHeight="1">
-      <c r="C125" s="8"/>
+      <c r="C125" s="10"/>
     </row>
     <row r="126" ht="15.75" customHeight="1">
-      <c r="C126" s="8"/>
+      <c r="C126" s="10"/>
     </row>
     <row r="127" ht="15.75" customHeight="1">
-      <c r="C127" s="8"/>
+      <c r="C127" s="10"/>
     </row>
     <row r="128" ht="15.75" customHeight="1">
-      <c r="C128" s="8"/>
+      <c r="C128" s="10"/>
     </row>
     <row r="129" ht="15.75" customHeight="1">
-      <c r="C129" s="8"/>
+      <c r="C129" s="10"/>
     </row>
     <row r="130" ht="15.75" customHeight="1">
-      <c r="C130" s="8"/>
+      <c r="C130" s="10"/>
     </row>
     <row r="131" ht="15.75" customHeight="1">
-      <c r="C131" s="8"/>
+      <c r="C131" s="10"/>
     </row>
     <row r="132" ht="15.75" customHeight="1">
-      <c r="C132" s="8"/>
+      <c r="C132" s="10"/>
     </row>
     <row r="133" ht="15.75" customHeight="1">
-      <c r="C133" s="8"/>
+      <c r="C133" s="10"/>
     </row>
     <row r="134" ht="15.75" customHeight="1">
-      <c r="C134" s="8"/>
+      <c r="C134" s="10"/>
     </row>
     <row r="135" ht="15.75" customHeight="1">
-      <c r="C135" s="8"/>
+      <c r="C135" s="10"/>
     </row>
     <row r="136" ht="15.75" customHeight="1">
-      <c r="C136" s="8"/>
+      <c r="C136" s="10"/>
     </row>
     <row r="137" ht="15.75" customHeight="1">
-      <c r="C137" s="8"/>
+      <c r="C137" s="10"/>
     </row>
     <row r="138" ht="15.75" customHeight="1">
-      <c r="C138" s="8"/>
+      <c r="C138" s="10"/>
     </row>
     <row r="139" ht="15.75" customHeight="1">
-      <c r="C139" s="8"/>
+      <c r="C139" s="10"/>
     </row>
     <row r="140" ht="15.75" customHeight="1">
-      <c r="C140" s="8"/>
+      <c r="C140" s="10"/>
     </row>
     <row r="141" ht="15.75" customHeight="1">
-      <c r="C141" s="8"/>
+      <c r="C141" s="10"/>
     </row>
     <row r="142" ht="15.75" customHeight="1">
-      <c r="C142" s="8"/>
+      <c r="C142" s="10"/>
     </row>
     <row r="143" ht="15.75" customHeight="1">
-      <c r="C143" s="8"/>
+      <c r="C143" s="10"/>
     </row>
     <row r="144" ht="15.75" customHeight="1">
-      <c r="C144" s="8"/>
+      <c r="C144" s="10"/>
     </row>
     <row r="145" ht="15.75" customHeight="1">
-      <c r="C145" s="8"/>
+      <c r="C145" s="10"/>
     </row>
     <row r="146" ht="15.75" customHeight="1">
-      <c r="C146" s="8"/>
+      <c r="C146" s="10"/>
     </row>
     <row r="147" ht="15.75" customHeight="1">
-      <c r="C147" s="8"/>
+      <c r="C147" s="10"/>
     </row>
     <row r="148" ht="15.75" customHeight="1">
-      <c r="C148" s="8"/>
+      <c r="C148" s="10"/>
     </row>
     <row r="149" ht="15.75" customHeight="1">
-      <c r="C149" s="8"/>
+      <c r="C149" s="10"/>
     </row>
     <row r="150" ht="15.75" customHeight="1">
-      <c r="C150" s="8"/>
+      <c r="C150" s="10"/>
     </row>
     <row r="151" ht="15.75" customHeight="1">
-      <c r="C151" s="8"/>
+      <c r="C151" s="10"/>
     </row>
     <row r="152" ht="15.75" customHeight="1">
-      <c r="C152" s="8"/>
+      <c r="C152" s="10"/>
     </row>
     <row r="153" ht="15.75" customHeight="1">
-      <c r="C153" s="8"/>
+      <c r="C153" s="10"/>
     </row>
     <row r="154" ht="15.75" customHeight="1">
-      <c r="C154" s="8"/>
+      <c r="C154" s="10"/>
     </row>
     <row r="155" ht="15.75" customHeight="1">
-      <c r="C155" s="8"/>
+      <c r="C155" s="10"/>
     </row>
     <row r="156" ht="15.75" customHeight="1">
-      <c r="C156" s="8"/>
+      <c r="C156" s="10"/>
     </row>
     <row r="157" ht="15.75" customHeight="1">
-      <c r="C157" s="8"/>
+      <c r="C157" s="10"/>
     </row>
     <row r="158" ht="15.75" customHeight="1">
-      <c r="C158" s="8"/>
+      <c r="C158" s="10"/>
     </row>
     <row r="159" ht="15.75" customHeight="1">
-      <c r="C159" s="8"/>
+      <c r="C159" s="10"/>
     </row>
     <row r="160" ht="15.75" customHeight="1">
-      <c r="C160" s="8"/>
+      <c r="C160" s="10"/>
     </row>
     <row r="161" ht="15.75" customHeight="1">
-      <c r="C161" s="8"/>
+      <c r="C161" s="10"/>
     </row>
     <row r="162" ht="15.75" customHeight="1">
-      <c r="C162" s="8"/>
+      <c r="C162" s="10"/>
     </row>
     <row r="163" ht="15.75" customHeight="1">
-      <c r="C163" s="8"/>
+      <c r="C163" s="10"/>
     </row>
     <row r="164" ht="15.75" customHeight="1">
-      <c r="C164" s="8"/>
+      <c r="C164" s="10"/>
     </row>
     <row r="165" ht="15.75" customHeight="1">
-      <c r="C165" s="8"/>
+      <c r="C165" s="10"/>
     </row>
     <row r="166" ht="15.75" customHeight="1">
-      <c r="C166" s="8"/>
+      <c r="C166" s="10"/>
     </row>
     <row r="167" ht="15.75" customHeight="1">
-      <c r="C167" s="8"/>
+      <c r="C167" s="10"/>
     </row>
     <row r="168" ht="15.75" customHeight="1">
-      <c r="C168" s="8"/>
+      <c r="C168" s="10"/>
     </row>
     <row r="169" ht="15.75" customHeight="1">
-      <c r="C169" s="8"/>
+      <c r="C169" s="10"/>
     </row>
     <row r="170" ht="15.75" customHeight="1">
-      <c r="C170" s="8"/>
+      <c r="C170" s="10"/>
     </row>
     <row r="171" ht="15.75" customHeight="1">
-      <c r="C171" s="8"/>
+      <c r="C171" s="10"/>
     </row>
     <row r="172" ht="15.75" customHeight="1">
-      <c r="C172" s="8"/>
+      <c r="C172" s="10"/>
     </row>
     <row r="173" ht="15.75" customHeight="1">
-      <c r="C173" s="8"/>
+      <c r="C173" s="10"/>
     </row>
     <row r="174" ht="15.75" customHeight="1">
-      <c r="C174" s="8"/>
+      <c r="C174" s="10"/>
     </row>
     <row r="175" ht="15.75" customHeight="1">
-      <c r="C175" s="8"/>
+      <c r="C175" s="10"/>
     </row>
     <row r="176" ht="15.75" customHeight="1">
-      <c r="C176" s="8"/>
+      <c r="C176" s="10"/>
     </row>
     <row r="177" ht="15.75" customHeight="1">
-      <c r="C177" s="8"/>
+      <c r="C177" s="10"/>
     </row>
     <row r="178" ht="15.75" customHeight="1">
-      <c r="C178" s="8"/>
+      <c r="C178" s="10"/>
     </row>
     <row r="179" ht="15.75" customHeight="1">
-      <c r="C179" s="8"/>
+      <c r="C179" s="10"/>
     </row>
     <row r="180" ht="15.75" customHeight="1">
-      <c r="C180" s="8"/>
+      <c r="C180" s="10"/>
     </row>
     <row r="181" ht="15.75" customHeight="1">
-      <c r="C181" s="8"/>
+      <c r="C181" s="10"/>
     </row>
     <row r="182" ht="15.75" customHeight="1">
-      <c r="C182" s="8"/>
+      <c r="C182" s="10"/>
     </row>
     <row r="183" ht="15.75" customHeight="1">
-      <c r="C183" s="8"/>
+      <c r="C183" s="10"/>
     </row>
     <row r="184" ht="15.75" customHeight="1">
-      <c r="C184" s="8"/>
+      <c r="C184" s="10"/>
     </row>
     <row r="185" ht="15.75" customHeight="1">
-      <c r="C185" s="8"/>
+      <c r="C185" s="10"/>
     </row>
     <row r="186" ht="15.75" customHeight="1">
-      <c r="C186" s="8"/>
+      <c r="C186" s="10"/>
     </row>
     <row r="187" ht="15.75" customHeight="1">
-      <c r="C187" s="8"/>
+      <c r="C187" s="10"/>
     </row>
     <row r="188" ht="15.75" customHeight="1">
-      <c r="C188" s="8"/>
+      <c r="C188" s="10"/>
     </row>
     <row r="189" ht="15.75" customHeight="1">
-      <c r="C189" s="8"/>
+      <c r="C189" s="10"/>
     </row>
     <row r="190" ht="15.75" customHeight="1">
-      <c r="C190" s="8"/>
+      <c r="C190" s="10"/>
     </row>
     <row r="191" ht="15.75" customHeight="1">
-      <c r="C191" s="8"/>
+      <c r="C191" s="10"/>
     </row>
     <row r="192" ht="15.75" customHeight="1">
-      <c r="C192" s="8"/>
+      <c r="C192" s="10"/>
     </row>
     <row r="193" ht="15.75" customHeight="1">
-      <c r="C193" s="8"/>
+      <c r="C193" s="10"/>
     </row>
     <row r="194" ht="15.75" customHeight="1">
-      <c r="C194" s="8"/>
+      <c r="C194" s="10"/>
     </row>
     <row r="195" ht="15.75" customHeight="1">
-      <c r="C195" s="8"/>
+      <c r="C195" s="10"/>
     </row>
     <row r="196" ht="15.75" customHeight="1">
-      <c r="C196" s="8"/>
+      <c r="C196" s="10"/>
     </row>
     <row r="197" ht="15.75" customHeight="1">
-      <c r="C197" s="8"/>
+      <c r="C197" s="10"/>
     </row>
     <row r="198" ht="15.75" customHeight="1">
-      <c r="C198" s="8"/>
+      <c r="C198" s="10"/>
     </row>
     <row r="199" ht="15.75" customHeight="1">
-      <c r="C199" s="8"/>
+      <c r="C199" s="10"/>
     </row>
     <row r="200" ht="15.75" customHeight="1">
-      <c r="C200" s="8"/>
+      <c r="C200" s="10"/>
     </row>
     <row r="201" ht="15.75" customHeight="1">
-      <c r="C201" s="8"/>
+      <c r="C201" s="10"/>
     </row>
     <row r="202" ht="15.75" customHeight="1">
-      <c r="C202" s="8"/>
+      <c r="C202" s="10"/>
     </row>
     <row r="203" ht="15.75" customHeight="1">
-      <c r="C203" s="8"/>
+      <c r="C203" s="10"/>
     </row>
     <row r="204" ht="15.75" customHeight="1">
-      <c r="C204" s="8"/>
+      <c r="C204" s="10"/>
     </row>
     <row r="205" ht="15.75" customHeight="1">
-      <c r="C205" s="8"/>
+      <c r="C205" s="10"/>
     </row>
     <row r="206" ht="15.75" customHeight="1">
-      <c r="C206" s="8"/>
+      <c r="C206" s="10"/>
     </row>
     <row r="207" ht="15.75" customHeight="1">
-      <c r="C207" s="8"/>
+      <c r="C207" s="10"/>
     </row>
     <row r="208" ht="15.75" customHeight="1">
-      <c r="C208" s="8"/>
+      <c r="C208" s="10"/>
     </row>
     <row r="209" ht="15.75" customHeight="1">
-      <c r="C209" s="8"/>
+      <c r="C209" s="10"/>
     </row>
     <row r="210" ht="15.75" customHeight="1">
-      <c r="C210" s="8"/>
+      <c r="C210" s="10"/>
     </row>
     <row r="211" ht="15.75" customHeight="1">
-      <c r="C211" s="8"/>
+      <c r="C211" s="10"/>
     </row>
     <row r="212" ht="15.75" customHeight="1">
-      <c r="C212" s="8"/>
+      <c r="C212" s="10"/>
     </row>
     <row r="213" ht="15.75" customHeight="1">
-      <c r="C213" s="8"/>
+      <c r="C213" s="10"/>
     </row>
     <row r="214" ht="15.75" customHeight="1">
-      <c r="C214" s="8"/>
+      <c r="C214" s="10"/>
     </row>
     <row r="215" ht="15.75" customHeight="1">
-      <c r="C215" s="8"/>
+      <c r="C215" s="10"/>
     </row>
     <row r="216" ht="15.75" customHeight="1">
-      <c r="C216" s="8"/>
+      <c r="C216" s="10"/>
     </row>
     <row r="217" ht="15.75" customHeight="1">
-      <c r="C217" s="8"/>
+      <c r="C217" s="10"/>
     </row>
     <row r="218" ht="15.75" customHeight="1">
-      <c r="C218" s="8"/>
+      <c r="C218" s="10"/>
     </row>
     <row r="219" ht="15.75" customHeight="1">
-      <c r="C219" s="8"/>
+      <c r="C219" s="10"/>
     </row>
     <row r="220" ht="15.75" customHeight="1">
-      <c r="C220" s="8"/>
+      <c r="C220" s="10"/>
     </row>
     <row r="221" ht="15.75" customHeight="1"/>
     <row r="222" ht="15.75" customHeight="1"/>
@@ -9725,7 +9836,7 @@
     <col customWidth="1" min="1" max="1" width="13.63"/>
     <col customWidth="1" min="2" max="2" width="11.88"/>
     <col customWidth="1" min="3" max="3" width="46.5"/>
-    <col customWidth="1" min="4" max="4" width="56.25"/>
+    <col customWidth="1" min="4" max="4" width="76.88"/>
     <col customWidth="1" min="5" max="6" width="12.63"/>
   </cols>
   <sheetData>
@@ -9734,7 +9845,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>2</v>
@@ -9767,13 +9878,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="20" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="D2" s="23">
         <v>9.9482454098E10</v>
@@ -9803,16 +9914,16 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="21" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -9839,16 +9950,16 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="21" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
@@ -9875,16 +9986,16 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="21" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -9911,16 +10022,16 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="21" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -9947,16 +10058,16 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="21" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
@@ -9983,16 +10094,16 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="21" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -10019,16 +10130,16 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="21" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -10054,10 +10165,18 @@
       <c r="Z9" s="3"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="26"/>
+      <c r="A10" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="25"/>

</xml_diff>